<commit_message>
Troubleshooting PyBank, skeleton for PyPoll
</commit_message>
<xml_diff>
--- a/PyBank/Resources/budget_data.xlsx
+++ b/PyBank/Resources/budget_data.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0d949fffeeafd9ab/Documents/GitHub/python-challenge/PyBank/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="18" documentId="8_{9ABAD32D-2FBC-4C0E-A070-97885D561C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{31690D3F-DF84-45A1-A1C5-E31010D2C070}"/>
+  <xr:revisionPtr revIDLastSave="31" documentId="8_{9ABAD32D-2FBC-4C0E-A070-97885D561C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FA82C76-4B31-4368-B0C9-7B9288A7C575}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="7380" yWindow="555" windowWidth="14355" windowHeight="14985" xr2:uid="{215A8E4D-3C0D-4B0D-A3EB-527A4A21B770}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{215A8E4D-3C0D-4B0D-A3EB-527A4A21B770}"/>
   </bookViews>
   <sheets>
     <sheet name="budget_data" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -34,7 +47,16 @@
     <t>Total Profits</t>
   </si>
   <si>
-    <t>Average Profit</t>
+    <t>Average Change</t>
+  </si>
+  <si>
+    <t>Change</t>
+  </si>
+  <si>
+    <t>Greatest Increase</t>
+  </si>
+  <si>
+    <t>Greatest Decrease</t>
   </si>
 </sst>
 </file>
@@ -897,733 +919,1090 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BBBC4AFC-F6D8-462E-9742-8E4B9E88E2C5}">
-  <dimension ref="A1:E87"/>
+  <dimension ref="A1:F87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="2">
+      <c r="F1" s="2">
         <f>COUNTA(A2:A87)</f>
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>45301</v>
       </c>
       <c r="B2">
         <v>1088983</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="2">
+      <c r="F2" s="2">
         <f>SUM(B2:B87)</f>
         <v>22564198</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>45332</v>
       </c>
       <c r="B3">
         <v>-354534</v>
       </c>
-      <c r="D3" t="s">
+      <c r="C3">
+        <f>B3-B2</f>
+        <v>-1443517</v>
+      </c>
+      <c r="E3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="2">
-        <f>AVERAGE(B2:B87)</f>
-        <v>262374.39534883719</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="2">
+        <f>AVERAGE(C3:C87)</f>
+        <v>-8311.105882352942</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>45361</v>
       </c>
       <c r="B4">
         <v>276622</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C4">
+        <f t="shared" ref="C4:C67" si="0">B4-B3</f>
+        <v>631156</v>
+      </c>
+      <c r="E4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="2">
+        <f>MAX(C3:C87)</f>
+        <v>1862002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>45392</v>
       </c>
       <c r="B5">
         <v>-728133</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>-1004755</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2">
+        <f>MIN(C3,C87)</f>
+        <v>-1443517</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>45422</v>
       </c>
       <c r="B6">
         <v>852993</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>1581126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>45453</v>
       </c>
       <c r="B7">
         <v>563721</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>-289272</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>45483</v>
       </c>
       <c r="B8">
         <v>-535208</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>-1098929</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>45514</v>
       </c>
       <c r="B9">
         <v>632349</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>1167557</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>45545</v>
       </c>
       <c r="B10">
         <v>-173744</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>-806093</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>45575</v>
       </c>
       <c r="B11">
         <v>950741</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>1124485</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>45606</v>
       </c>
       <c r="B12">
         <v>-785750</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>-1736491</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>45636</v>
       </c>
       <c r="B13">
         <v>-1194133</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <f t="shared" si="0"/>
+        <v>-408383</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>45302</v>
       </c>
       <c r="B14">
         <v>-589576</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <f t="shared" si="0"/>
+        <v>604557</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>45333</v>
       </c>
       <c r="B15">
         <v>-883921</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <f t="shared" si="0"/>
+        <v>-294345</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>45362</v>
       </c>
       <c r="B16">
         <v>443564</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C16">
+        <f t="shared" si="0"/>
+        <v>1327485</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>45393</v>
       </c>
       <c r="B17">
         <v>837887</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C17">
+        <f t="shared" si="0"/>
+        <v>394323</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>45423</v>
       </c>
       <c r="B18">
         <v>1081472</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C18">
+        <f t="shared" si="0"/>
+        <v>243585</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>45454</v>
       </c>
       <c r="B19">
         <v>464033</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C19">
+        <f t="shared" si="0"/>
+        <v>-617439</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>45484</v>
       </c>
       <c r="B20">
         <v>-1066544</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C20">
+        <f t="shared" si="0"/>
+        <v>-1530577</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>45515</v>
       </c>
       <c r="B21">
         <v>323846</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C21">
+        <f t="shared" si="0"/>
+        <v>1390390</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>45546</v>
       </c>
       <c r="B22">
         <v>-806551</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C22">
+        <f t="shared" si="0"/>
+        <v>-1130397</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>45576</v>
       </c>
       <c r="B23">
         <v>487053</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C23">
+        <f t="shared" si="0"/>
+        <v>1293604</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>45607</v>
       </c>
       <c r="B24">
         <v>1128811</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C24">
+        <f t="shared" si="0"/>
+        <v>641758</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>45637</v>
       </c>
       <c r="B25">
         <v>791398</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C25">
+        <f t="shared" si="0"/>
+        <v>-337413</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>45303</v>
       </c>
       <c r="B26">
         <v>739367</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C26">
+        <f t="shared" si="0"/>
+        <v>-52031</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>45334</v>
       </c>
       <c r="B27">
         <v>-197825</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <f t="shared" si="0"/>
+        <v>-937192</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>45363</v>
       </c>
       <c r="B28">
         <v>666016</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C28">
+        <f t="shared" si="0"/>
+        <v>863841</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>45394</v>
       </c>
       <c r="B29">
         <v>589771</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C29">
+        <f t="shared" si="0"/>
+        <v>-76245</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>45424</v>
       </c>
       <c r="B30">
         <v>489290</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C30">
+        <f t="shared" si="0"/>
+        <v>-100481</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>45455</v>
       </c>
       <c r="B31">
         <v>-471439</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C31">
+        <f t="shared" si="0"/>
+        <v>-960729</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>45485</v>
       </c>
       <c r="B32">
         <v>120417</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C32">
+        <f t="shared" si="0"/>
+        <v>591856</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>45516</v>
       </c>
       <c r="B33">
         <v>175347</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C33">
+        <f t="shared" si="0"/>
+        <v>54930</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>45547</v>
       </c>
       <c r="B34">
         <v>855449</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34">
+        <f t="shared" si="0"/>
+        <v>680102</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>45577</v>
       </c>
       <c r="B35">
         <v>605195</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C35">
+        <f t="shared" si="0"/>
+        <v>-250254</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>45608</v>
       </c>
       <c r="B36">
         <v>-235220</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C36">
+        <f t="shared" si="0"/>
+        <v>-840415</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>45638</v>
       </c>
       <c r="B37">
         <v>347138</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C37">
+        <f t="shared" si="0"/>
+        <v>582358</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>45304</v>
       </c>
       <c r="B38">
         <v>298510</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C38">
+        <f t="shared" si="0"/>
+        <v>-48628</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>45335</v>
       </c>
       <c r="B39">
         <v>163254</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C39">
+        <f t="shared" si="0"/>
+        <v>-135256</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>45364</v>
       </c>
       <c r="B40">
         <v>1141840</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C40">
+        <f t="shared" si="0"/>
+        <v>978586</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>45395</v>
       </c>
       <c r="B41">
         <v>542630</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C41">
+        <f t="shared" si="0"/>
+        <v>-599210</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>45425</v>
       </c>
       <c r="B42">
         <v>99841</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C42">
+        <f t="shared" si="0"/>
+        <v>-442789</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>45456</v>
       </c>
       <c r="B43">
         <v>752765</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C43">
+        <f t="shared" si="0"/>
+        <v>652924</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>45486</v>
       </c>
       <c r="B44">
         <v>-252949</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C44">
+        <f t="shared" si="0"/>
+        <v>-1005714</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>45517</v>
       </c>
       <c r="B45">
         <v>914424</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C45">
+        <f t="shared" si="0"/>
+        <v>1167373</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>45548</v>
       </c>
       <c r="B46">
         <v>679524</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C46">
+        <f t="shared" si="0"/>
+        <v>-234900</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>45578</v>
       </c>
       <c r="B47">
         <v>514377</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C47">
+        <f t="shared" si="0"/>
+        <v>-165147</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>45609</v>
       </c>
       <c r="B48">
         <v>462102</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C48">
+        <f t="shared" si="0"/>
+        <v>-52275</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>45639</v>
       </c>
       <c r="B49">
         <v>159782</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C49">
+        <f t="shared" si="0"/>
+        <v>-302320</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>45305</v>
       </c>
       <c r="B50">
         <v>878810</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C50">
+        <f t="shared" si="0"/>
+        <v>719028</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>45336</v>
       </c>
       <c r="B51">
         <v>-946748</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C51">
+        <f t="shared" si="0"/>
+        <v>-1825558</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>45365</v>
       </c>
       <c r="B52">
         <v>340335</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C52">
+        <f t="shared" si="0"/>
+        <v>1287083</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>45396</v>
       </c>
       <c r="B53">
         <v>292032</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C53">
+        <f t="shared" si="0"/>
+        <v>-48303</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>45426</v>
       </c>
       <c r="B54">
         <v>502266</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C54">
+        <f t="shared" si="0"/>
+        <v>210234</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>45457</v>
       </c>
       <c r="B55">
         <v>265852</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C55">
+        <f t="shared" si="0"/>
+        <v>-236414</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>45487</v>
       </c>
       <c r="B56">
         <v>851017</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C56">
+        <f t="shared" si="0"/>
+        <v>585165</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>45518</v>
       </c>
       <c r="B57">
         <v>-549615</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C57">
+        <f t="shared" si="0"/>
+        <v>-1400632</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>45549</v>
       </c>
       <c r="B58">
         <v>290162</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C58">
+        <f t="shared" si="0"/>
+        <v>839777</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>45579</v>
       </c>
       <c r="B59">
         <v>755391</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C59">
+        <f t="shared" si="0"/>
+        <v>465229</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>45610</v>
       </c>
       <c r="B60">
         <v>1073202</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C60">
+        <f t="shared" si="0"/>
+        <v>317811</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>45640</v>
       </c>
       <c r="B61">
         <v>313000</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C61">
+        <f t="shared" si="0"/>
+        <v>-760202</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>45306</v>
       </c>
       <c r="B62">
         <v>241132</v>
       </c>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C62">
+        <f t="shared" si="0"/>
+        <v>-71868</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>45337</v>
       </c>
       <c r="B63">
         <v>1036589</v>
       </c>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C63">
+        <f t="shared" si="0"/>
+        <v>795457</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>45366</v>
       </c>
       <c r="B64">
         <v>853904</v>
       </c>
-    </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C64">
+        <f t="shared" si="0"/>
+        <v>-182685</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>45397</v>
       </c>
       <c r="B65">
         <v>-388932</v>
       </c>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C65">
+        <f t="shared" si="0"/>
+        <v>-1242836</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>45427</v>
       </c>
       <c r="B66">
         <v>982952</v>
       </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C66">
+        <f t="shared" si="0"/>
+        <v>1371884</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>45458</v>
       </c>
       <c r="B67">
         <v>537759</v>
       </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C67">
+        <f t="shared" si="0"/>
+        <v>-445193</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>45488</v>
       </c>
       <c r="B68">
         <v>547784</v>
       </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C68">
+        <f t="shared" ref="C68:C87" si="1">B68-B67</f>
+        <v>10025</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>45519</v>
       </c>
       <c r="B69">
         <v>-496214</v>
       </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C69">
+        <f t="shared" si="1"/>
+        <v>-1043998</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>45550</v>
       </c>
       <c r="B70">
         <v>854181</v>
       </c>
-    </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C70">
+        <f t="shared" si="1"/>
+        <v>1350395</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>45580</v>
       </c>
       <c r="B71">
         <v>934719</v>
       </c>
-    </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C71">
+        <f t="shared" si="1"/>
+        <v>80538</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>45611</v>
       </c>
       <c r="B72">
         <v>-288531</v>
       </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C72">
+        <f t="shared" si="1"/>
+        <v>-1223250</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>45641</v>
       </c>
       <c r="B73">
         <v>-184383</v>
       </c>
-    </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C73">
+        <f t="shared" si="1"/>
+        <v>104148</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>45307</v>
       </c>
       <c r="B74">
         <v>659541</v>
       </c>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C74">
+        <f t="shared" si="1"/>
+        <v>843924</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>45338</v>
       </c>
       <c r="B75">
         <v>-1149123</v>
       </c>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C75">
+        <f t="shared" si="1"/>
+        <v>-1808664</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>45367</v>
       </c>
       <c r="B76">
         <v>355882</v>
       </c>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C76">
+        <f t="shared" si="1"/>
+        <v>1505005</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>45398</v>
       </c>
       <c r="B77">
         <v>662284</v>
       </c>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C77">
+        <f t="shared" si="1"/>
+        <v>306402</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>45428</v>
       </c>
       <c r="B78">
         <v>518681</v>
       </c>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C78">
+        <f t="shared" si="1"/>
+        <v>-143603</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>45459</v>
       </c>
       <c r="B79">
         <v>-748256</v>
       </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C79">
+        <f t="shared" si="1"/>
+        <v>-1266937</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>45489</v>
       </c>
       <c r="B80">
         <v>-910775</v>
       </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C80">
+        <f t="shared" si="1"/>
+        <v>-162519</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>45520</v>
       </c>
       <c r="B81">
         <v>951227</v>
       </c>
-    </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C81">
+        <f t="shared" si="1"/>
+        <v>1862002</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>45551</v>
       </c>
       <c r="B82">
         <v>898241</v>
       </c>
-    </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C82">
+        <f t="shared" si="1"/>
+        <v>-52986</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>45581</v>
       </c>
       <c r="B83">
         <v>-729004</v>
       </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C83">
+        <f t="shared" si="1"/>
+        <v>-1627245</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>45612</v>
       </c>
       <c r="B84">
         <v>-112209</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C84">
+        <f t="shared" si="1"/>
+        <v>616795</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>45642</v>
       </c>
       <c r="B85">
         <v>516313</v>
       </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C85">
+        <f t="shared" si="1"/>
+        <v>628522</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>45308</v>
       </c>
       <c r="B86">
         <v>607208</v>
       </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C86">
+        <f t="shared" si="1"/>
+        <v>90895</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>45339</v>
       </c>
       <c r="B87">
         <v>382539</v>
+      </c>
+      <c r="C87">
+        <f t="shared" si="1"/>
+        <v>-224669</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PyBank moved to two loops for input and calc
</commit_message>
<xml_diff>
--- a/PyBank/Resources/budget_data.xlsx
+++ b/PyBank/Resources/budget_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/0d949fffeeafd9ab/Documents/GitHub/python-challenge/PyBank/Resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="31" documentId="8_{9ABAD32D-2FBC-4C0E-A070-97885D561C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5FA82C76-4B31-4368-B0C9-7B9288A7C575}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="8_{9ABAD32D-2FBC-4C0E-A070-97885D561C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3BF47C9A-1836-4736-98A1-7B6DED23490F}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{215A8E4D-3C0D-4B0D-A3EB-527A4A21B770}"/>
+    <workbookView minimized="1" xWindow="3120" yWindow="1215" windowWidth="14355" windowHeight="14985" xr2:uid="{215A8E4D-3C0D-4B0D-A3EB-527A4A21B770}"/>
   </bookViews>
   <sheets>
     <sheet name="budget_data" sheetId="1" r:id="rId1"/>
@@ -922,7 +922,7 @@
   <dimension ref="A1:F87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>